<commit_message>
[fix] Fix column trimming method
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,26 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9180"/>
+    <workbookView windowWidth="23040" windowHeight="9144"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="settings" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -172,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -183,7 +170,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -191,7 +178,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -199,7 +186,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -207,14 +194,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -222,7 +209,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -230,7 +217,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -238,7 +225,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -246,7 +233,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -254,14 +241,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -269,7 +256,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -277,7 +264,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -285,14 +272,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -300,42 +287,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -828,55 +815,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1486,7 +1473,9 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>

</xml_diff>